<commit_message>
Updates to drug methodology.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\test\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44130D28-B26B-48FC-A400-B46994DBD541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAAD2D9-4909-47CA-A53B-6769C6341D45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17400" yWindow="5220" windowWidth="32670" windowHeight="23535" tabRatio="736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3975" yWindow="2895" windowWidth="24825" windowHeight="11385" tabRatio="736" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="18" r:id="rId1"/>
@@ -27,7 +27,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="120">
   <si>
     <t>Event</t>
   </si>
@@ -384,9 +387,6 @@
   </si>
   <si>
     <t>Decrease ~15% @cite mancebo1991effects</t>
-  </si>
-  <si>
-    <t>|&lt;span class="warning"&gt;</t>
   </si>
   <si>
     <t>Administer 10 ug injection of Epinephrine</t>
@@ -1585,8 +1585,8 @@
   </sheetPr>
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,7 +1725,7 @@
         <v>52</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" s="65" t="s">
         <v>54</v>
@@ -1955,7 +1955,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E10" s="65" t="s">
         <v>54</v>
@@ -2169,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,8 +2248,8 @@
   </sheetPr>
   <dimension ref="A2:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2297,7 +2297,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>52</v>
@@ -2577,8 +2577,8 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection activeCell="B15" sqref="A1:XFD1048576"/>
-      <selection pane="topRight" activeCell="B15" sqref="A1:XFD1048576"/>
+      <selection activeCell="F4" sqref="F4"/>
+      <selection pane="topRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +2624,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" s="42" t="s">
         <v>52</v>
@@ -2751,9 +2751,9 @@
         <v>150</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="J4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="15" t="s">
         <v>71</v>
       </c>
       <c r="K4" s="42" t="s">
@@ -2996,13 +2996,13 @@
         <v>64</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M8" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O8" s="42" t="s">
         <v>64</v>
@@ -3379,7 +3379,7 @@
         <v>52</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>52</v>
@@ -3442,8 +3442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3501,7 +3501,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Fixed tables in the drug methodology report.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngineStable\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F0217-02D9-4613-AB36-590F8224060B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3702991-10C0-4105-A61C-932E040DF8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="736" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="175">
   <si>
     <t>Event</t>
   </si>
@@ -418,12 +418,6 @@
     <t>Little Respiratory Depression @cite Valk2021etomidate</t>
   </si>
   <si>
-    <t>Experimental           Plasma Concentration (ug/L)</t>
-  </si>
-  <si>
-    <t>Computed              Plasma Concentration  (ug/L)</t>
-  </si>
-  <si>
     <t>Drug</t>
   </si>
   <si>
@@ -448,93 +442,6 @@
     <t>[6.404, 8.546] @cite ensinger1992relationship</t>
   </si>
   <si>
-    <t>Experimental           Heart Rate 
-(beats/min)</t>
-  </si>
-  <si>
-    <t>Computed         
-     Heart Rate
- (beats/min)</t>
-  </si>
-  <si>
-    <t>Experimental           Systolic Blood Pressure
-(mmHg)</t>
-  </si>
-  <si>
-    <t>Computed         
-    Systolic Blood Pressure
-(mmHg)</t>
-  </si>
-  <si>
-    <t>Experimental           Diastolic Blood Pressure
-(mmHg)</t>
-  </si>
-  <si>
-    <t>Computed         
-    Diastolic Blood Pressure
-(mmHg)</t>
-  </si>
-  <si>
-    <t>[46, 66] 
-NC to neglible @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[41, 57]
-Minimal Decrease @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[40, 56] 
-Minimal Decrease @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[39, 55] 
-Minimal Decrease@cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[39, 55] 
-NC @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[125, 145]
-Minimal Increase @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[136, 160] 
-Minimal Increase @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[146, 168] 
-Minimal Increase @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[152, 182] 
-Minimal Increase @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[174, 192] 
-Minimal Increase @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[65, 75] 
-NC @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[70, 84] 
-Minimal Increase @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[74, 86] 
-Minimal Increase @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[77, 93] 
-Minimal Increase @cite ensinger1992relationship</t>
-  </si>
-  <si>
-    <t>[83, 99] 
-Minimal Increase @cite ensinger1992relationship</t>
-  </si>
-  <si>
     <t>Phenylephrine</t>
   </si>
   <si>
@@ -550,61 +457,118 @@
     <t>[35.6, 77.8] @cite martinsson1986analysis</t>
   </si>
   <si>
-    <t>Experimental           Heart Rate Change
-(beats/min)</t>
-  </si>
-  <si>
-    <t>Computed         
-     Heart Rate Change
- (beats/min)</t>
-  </si>
-  <si>
-    <t>[0, 6]
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[6, 20]
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[16, 53]
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[30, 86]
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[2, 9]
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[9, 15]
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[15, 21]
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[25, 32]
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[1, -5] 
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[-3, -8] 
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[-8, -12] 
- @cite martinsson1986analysis</t>
-  </si>
-  <si>
-    <t>[-10, -13] 
- @cite martinsson1986analysis</t>
+    <t>Experimental Plasma Concentration (ug/L)</t>
+  </si>
+  <si>
+    <t>Computed Plasma Concentration (ug/L)</t>
+  </si>
+  <si>
+    <t>Experimental Heart Rate (beats/min)</t>
+  </si>
+  <si>
+    <t>Computed Heart Rate (beats/min)</t>
+  </si>
+  <si>
+    <t>Experimental Systolic Blood Pressure (mmHg)</t>
+  </si>
+  <si>
+    <t>Computed Systolic Blood Pressure (mmHg)</t>
+  </si>
+  <si>
+    <t>Experimental Diastolic Blood Pressure (mmHg)</t>
+  </si>
+  <si>
+    <t>Computed Diastolic Blood Pressure (mmHg)</t>
+  </si>
+  <si>
+    <t>[136, 160]  Minimal Increase @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[146, 168]  Minimal Increase @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[152, 182]  Minimal Increase @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[174, 192]  Minimal Increase @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[70, 84]  Minimal Increase @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[74, 86] Minimal Increase @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[77, 93] Minimal Increase @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[83, 99] Minimal Increase @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[39, 55] NC @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[39, 55] Minimal Decrease@cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[40, 56] Minimal Decrease @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[41, 57]Minimal Decrease @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[2, 9] @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[9, 15] @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[15, 21] @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[25, 32] @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[30, 86] @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[16, 53] @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[6, 20] @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[0, 6] @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[1, -5]  @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[-3, -8]  @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[-8, -12]  @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>[-10, -13]  @cite martinsson1986analysis</t>
+  </si>
+  <si>
+    <t>|&lt;span class="warning"&gt;</t>
+  </si>
+  <si>
+    <t>[46, 66] NC to neglible @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[125, 145] Minimal Increase @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>[65, 75] NC @cite ensinger1992relationship</t>
+  </si>
+  <si>
+    <t>Computed Heart Rate Change (beats/min)</t>
+  </si>
+  <si>
+    <t>Experimental Heart Rate Change (beats/min)</t>
   </si>
 </sst>
 </file>
@@ -2782,9 +2746,9 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection activeCell="F4" sqref="F4"/>
-      <selection pane="topRight" activeCell="K4" sqref="K4"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,7 +2763,7 @@
     <col min="8" max="8" width="23.5703125" style="74" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.7109375" style="36" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.7109375" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" style="36" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" customWidth="1"/>
     <col min="13" max="13" width="29.7109375" style="36" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="36.7109375" customWidth="1"/>
@@ -2997,13 +2961,27 @@
       <c r="B5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="42"/>
+      <c r="C5" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="1">
+        <v>30</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="3">
+        <v>100</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>54</v>
+      </c>
       <c r="J5" s="15" t="s">
         <v>122</v>
       </c>
@@ -3691,10 +3669,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D4665F2-3693-4E72-BE85-0371B19A8C03}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3706,21 +3684,21 @@
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="30.42578125" customWidth="1"/>
     <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="24" customWidth="1"/>
     <col min="12" max="12" width="23.140625" customWidth="1"/>
-    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.7109375" customWidth="1"/>
     <col min="15" max="15" width="25.42578125" customWidth="1"/>
     <col min="16" max="16" width="23" customWidth="1"/>
-    <col min="17" max="17" width="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" customWidth="1"/>
+    <col min="19" max="19" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="53"/>
       <c r="B1" s="53"/>
       <c r="E1" s="53"/>
@@ -3736,136 +3714,142 @@
       <c r="S1" s="53"/>
       <c r="T1" s="53"/>
     </row>
-    <row r="2" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="E2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="G2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="O2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="S2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="S3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="I2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="K2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="M2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="O2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="S2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="O3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="P3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="R3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="S3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>52</v>
@@ -3877,57 +3861,60 @@
         <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="H4" s="12">
         <v>0.76100000000000001</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>52</v>
+      <c r="I4" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="L4" s="15">
         <v>73</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>52</v>
+      <c r="M4" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="O4" s="42" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="P4" s="12">
         <v>118</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>52</v>
+      <c r="Q4" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="T4" s="12">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="U4" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>52</v>
@@ -3939,57 +3926,60 @@
         <v>52</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H5" s="15">
         <v>2.3199999999999998</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>52</v>
+      <c r="I5" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="K5" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="L5" s="15">
         <v>70</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>52</v>
+      <c r="M5" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O5" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="P5" s="15">
         <v>118</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>52</v>
+      <c r="Q5" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S5" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="T5" s="15">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="U5" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>52</v>
@@ -4001,55 +3991,60 @@
         <v>52</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H6" s="15">
         <v>3.71</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>52</v>
+      <c r="I6" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="L6" s="15">
         <v>68</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>52</v>
+      <c r="M6" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O6" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="P6" s="15">
         <v>125</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>52</v>
+      <c r="Q6" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="S6" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="T6" s="15">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="U6" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>52</v>
@@ -4061,55 +4056,60 @@
         <v>52</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H7" s="15">
         <v>5.05</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>52</v>
+      <c r="I7" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="L7" s="15">
         <v>69</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>52</v>
+      <c r="M7" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="P7" s="15">
         <v>135</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>52</v>
+      <c r="Q7" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="S7" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="T7" s="15">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="U7" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>52</v>
@@ -4121,49 +4121,52 @@
         <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G8" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H8" s="15">
         <v>7.1</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>52</v>
+      <c r="I8" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="L8" s="15">
         <v>69</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>52</v>
+      <c r="M8" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O8" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="P8" s="15">
         <v>136</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>52</v>
+      <c r="Q8" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="S8" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="T8" s="15">
         <v>100</v>
+      </c>
+      <c r="U8" s="40" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -4174,10 +4177,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D12168-200B-46C7-8F89-55DD217C0DF8}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:T7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4190,87 +4193,90 @@
     <col min="6" max="6" width="22.42578125" style="53" customWidth="1"/>
     <col min="7" max="7" width="30.42578125" style="53" customWidth="1"/>
     <col min="8" max="8" width="21.140625" style="53" customWidth="1"/>
-    <col min="9" max="9" width="2" style="53" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="53" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" style="53" customWidth="1"/>
     <col min="11" max="11" width="24" style="53" customWidth="1"/>
     <col min="12" max="12" width="23.140625" style="53" customWidth="1"/>
-    <col min="13" max="13" width="2" style="53" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="53" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.7109375" style="53" customWidth="1"/>
     <col min="15" max="15" width="25.42578125" style="53" customWidth="1"/>
     <col min="16" max="16" width="23" style="53" customWidth="1"/>
-    <col min="17" max="17" width="2" style="53" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" style="53" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23.5703125" style="53" customWidth="1"/>
     <col min="19" max="19" width="32.5703125" style="53" customWidth="1"/>
     <col min="20" max="20" width="28.28515625" style="53" customWidth="1"/>
     <col min="21" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F1" s="74"/>
     </row>
-    <row r="2" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="E2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="G2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="I2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="K2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="M2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="O2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="Q2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="S2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>52</v>
       </c>
@@ -4331,13 +4337,16 @@
       <c r="T3" s="24" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="U3" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>52</v>
@@ -4349,57 +4358,60 @@
         <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="H4" s="12">
         <v>6</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>52</v>
+      <c r="I4" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="L4" s="15">
         <v>-2</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>52</v>
+      <c r="M4" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="O4" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="P4" s="15">
         <v>6</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>52</v>
+      <c r="Q4" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="T4" s="15">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="U4" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>52</v>
@@ -4411,57 +4423,60 @@
         <v>52</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>54</v>
       </c>
       <c r="H5" s="15">
         <v>12.4</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>52</v>
+      <c r="I5" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="K5" s="42" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="L5" s="12">
         <v>-2</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>52</v>
+      <c r="M5" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>163</v>
       </c>
       <c r="O5" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="P5" s="15">
         <v>9</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>52</v>
+      <c r="Q5" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="S5" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="T5" s="15">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="U5" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>52</v>
@@ -4473,55 +4488,60 @@
         <v>52</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H6" s="15">
         <v>24.9</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>52</v>
+      <c r="I6" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="L6" s="73">
         <v>-1</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>52</v>
+      <c r="M6" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O6" s="42" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="P6" s="12">
         <v>13</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>52</v>
+      <c r="Q6" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="S6" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="T6" s="15">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="U6" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>52</v>
@@ -4533,50 +4553,56 @@
         <v>52</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H7" s="15">
         <v>48.4</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>52</v>
+      <c r="I7" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="L7" s="73">
         <v>2</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>52</v>
+      <c r="M7" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="P7" s="12">
         <v>17</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>52</v>
+      <c r="Q7" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="S7" s="42" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="T7" s="15">
         <v>25</v>
       </c>
+      <c r="U7" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U8" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4587,15 +4613,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Added Lorazepam and updated the drug methodology.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngineStable\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E22D66-F03A-4B4D-901D-5BDE2CD8356B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C569540-7DCA-4F52-88EA-07A31D239136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="Furosemide" sheetId="25" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$N$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$N$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="183">
   <si>
     <t>Event</t>
   </si>
@@ -575,6 +575,24 @@
   </si>
   <si>
     <t>Administer 21 ug injection of Etomidate</t>
+  </si>
+  <si>
+    <t>Lorazepam</t>
+  </si>
+  <si>
+    <t>Administer 2 mg injection of Lorazepam</t>
+  </si>
+  <si>
+    <t>Administer Lorazepam - 2 mg</t>
+  </si>
+  <si>
+    <t>Drug Onset &lt; 2 minutes</t>
+  </si>
+  <si>
+    <t>Mild Decrease @cite Tulen1991dose</t>
+  </si>
+  <si>
+    <t>Mild Decrease @cite Ghiasi2021lorazepam</t>
   </si>
 </sst>
 </file>
@@ -1759,10 +1777,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,18 +2064,18 @@
       <c r="N7" s="47"/>
       <c r="O7" s="47"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+    <row r="8" spans="1:15" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>177</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>178</v>
       </c>
       <c r="E8" s="65" t="s">
         <v>54</v>
@@ -2065,13 +2083,13 @@
       <c r="F8" s="10">
         <v>5</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="72" t="s">
         <v>98</v>
       </c>
       <c r="H8" s="8">
         <v>0</v>
       </c>
-      <c r="I8" s="71" t="s">
+      <c r="I8" s="72" t="s">
         <v>99</v>
       </c>
       <c r="J8" s="9">
@@ -2086,17 +2104,17 @@
       <c r="O8" s="47"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="48" t="s">
         <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="55" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" s="65" t="s">
         <v>54</v>
@@ -2124,18 +2142,18 @@
       <c r="N9" s="47"/>
       <c r="O9" s="47"/>
     </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="54" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>100</v>
+        <v>36</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="65" t="s">
         <v>54</v>
@@ -2158,19 +2176,23 @@
       <c r="K10" s="51" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="55" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C11" s="55" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="E11" s="65" t="s">
         <v>54</v>
@@ -2199,13 +2221,13 @@
         <v>52</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="55" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="E12" s="65" t="s">
         <v>54</v>
@@ -2213,13 +2235,13 @@
       <c r="F12" s="10">
         <v>5</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="G12" s="68" t="s">
         <v>98</v>
       </c>
       <c r="H12" s="8">
         <v>0</v>
       </c>
-      <c r="I12" s="72" t="s">
+      <c r="I12" s="71" t="s">
         <v>99</v>
       </c>
       <c r="J12" s="9">
@@ -2234,31 +2256,31 @@
         <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="C13" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>39</v>
+      <c r="D13" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E13" s="65" t="s">
         <v>54</v>
       </c>
       <c r="F13" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G13" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="8">
         <v>0</v>
       </c>
       <c r="I13" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="J13" s="17">
-        <v>1</v>
+      <c r="J13" s="9">
+        <v>0</v>
       </c>
       <c r="K13" s="51" t="s">
         <v>56</v>
@@ -2269,31 +2291,31 @@
         <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="55" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E14" s="65" t="s">
         <v>54</v>
       </c>
       <c r="F14" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G14" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="16">
         <v>0</v>
       </c>
       <c r="I14" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="J14" s="9">
-        <v>3</v>
+      <c r="J14" s="17">
+        <v>1</v>
       </c>
       <c r="K14" s="51" t="s">
         <v>56</v>
@@ -2304,19 +2326,19 @@
         <v>52</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="55" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="65" t="s">
         <v>54</v>
       </c>
       <c r="F15" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G15" s="69" t="s">
         <v>98</v>
@@ -2328,45 +2350,80 @@
         <v>99</v>
       </c>
       <c r="J15" s="9">
+        <v>3</v>
+      </c>
+      <c r="K15" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="10">
+        <v>5</v>
+      </c>
+      <c r="G16" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="8">
         <v>0</v>
       </c>
-      <c r="K15" s="51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="59" t="s">
+      <c r="I16" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+      <c r="K16" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="58"/>
+      <c r="C17" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="60">
-        <f>SUM(F3:F15)</f>
-        <v>59</v>
-      </c>
-      <c r="G16" s="61" t="s">
+      <c r="E17" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="60">
+        <f>SUM(F3:F16)</f>
+        <v>64</v>
+      </c>
+      <c r="G17" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="62">
-        <f>SUM(H3:H15)</f>
+      <c r="H17" s="62">
+        <f>SUM(H3:H16)</f>
         <v>2</v>
       </c>
-      <c r="I16" s="61" t="s">
+      <c r="I17" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="J16" s="63">
-        <f>SUM(J3:J15)</f>
+      <c r="J17" s="63">
+        <f>SUM(J3:J16)</f>
         <v>4</v>
       </c>
-      <c r="K16" s="64" t="s">
+      <c r="K17" s="64" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2788,12 +2845,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection activeCell="F4" sqref="F4"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:S16"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3176,60 +3233,60 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
+      <c r="B8" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
+      <c r="D8" s="42" t="s">
+        <v>180</v>
       </c>
       <c r="E8" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="42">
         <v>30</v>
       </c>
       <c r="G8" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="3">
-        <v>70</v>
+      <c r="H8" s="2">
+        <v>350</v>
       </c>
       <c r="I8" s="42" t="s">
         <v>54</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="K8" s="42" t="s">
         <v>64</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="M8" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="O8" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>89</v>
+        <v>182</v>
       </c>
       <c r="Q8" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="R8" s="13" t="s">
-        <v>102</v>
+      <c r="R8" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="S8" s="42" t="s">
         <v>56</v>
@@ -3240,13 +3297,13 @@
         <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E9" s="42" t="s">
         <v>52</v>
@@ -3258,31 +3315,31 @@
         <v>52</v>
       </c>
       <c r="H9" s="3">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I9" s="42" t="s">
         <v>54</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K9" s="42" t="s">
         <v>64</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="M9" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="O9" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q9" s="42" t="s">
         <v>64</v>
@@ -3299,13 +3356,13 @@
         <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E10" s="42" t="s">
         <v>52</v>
@@ -3323,149 +3380,149 @@
         <v>54</v>
       </c>
       <c r="J10" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="M10" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="O10" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="R10" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="S10" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="1">
+        <v>30</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="3">
+        <v>100</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L10" s="15" t="s">
+      <c r="K11" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N10" s="15" t="s">
+      <c r="M11" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N11" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="O10" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P10" s="15" t="s">
+      <c r="O11" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="P11" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="Q10" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="R10" s="14" t="s">
+      <c r="Q11" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="R11" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="S10" s="42" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="S11" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C12" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="E12" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1">
         <v>330</v>
       </c>
-      <c r="G11" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="G12" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="3">
         <v>350</v>
       </c>
-      <c r="I11" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="15" t="s">
+      <c r="I12" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L11" s="15" t="s">
+      <c r="K12" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="M11" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N11" s="15" t="s">
+      <c r="M12" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N12" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="O11" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P11" s="15" t="s">
+      <c r="O12" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="Q11" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="R11" s="15" t="s">
+      <c r="Q12" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="R12" s="15" t="s">
         <v>103</v>
-      </c>
-      <c r="S11" s="42" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="1">
-        <v>30</v>
-      </c>
-      <c r="G12" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="3">
-        <v>100</v>
-      </c>
-      <c r="I12" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="M12" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N12" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="O12" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="P12" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q12" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="R12" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="S12" s="42" t="s">
         <v>56</v>
@@ -3476,7 +3533,7 @@
         <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="42" t="s">
         <v>52</v>
@@ -3500,25 +3557,25 @@
         <v>54</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K13" s="42" t="s">
         <v>64</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M13" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O13" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P13" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q13" s="42" t="s">
         <v>64</v>
@@ -3530,12 +3587,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
         <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>52</v>
@@ -3556,51 +3613,51 @@
         <v>100</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="J14" s="73" t="s">
-        <v>81</v>
+        <v>54</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="K14" s="42" t="s">
         <v>64</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="M14" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="O14" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P14" s="15" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="Q14" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="R14" s="13" t="s">
-        <v>104</v>
+      <c r="R14" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="S14" s="42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>52</v>
@@ -3618,25 +3675,25 @@
         <v>59</v>
       </c>
       <c r="J15" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K15" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="L15" s="73" t="s">
-        <v>82</v>
+        <v>64</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>85</v>
       </c>
       <c r="M15" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="N15" s="73" t="s">
-        <v>82</v>
+        <v>64</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>85</v>
       </c>
       <c r="O15" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P15" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q15" s="42" t="s">
         <v>64</v>
@@ -3648,48 +3705,48 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="42" t="s">
-        <v>119</v>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="42" t="s">
-        <v>7</v>
+      <c r="D16" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="1">
         <v>30</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <v>100</v>
       </c>
       <c r="I16" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>83</v>
+        <v>59</v>
+      </c>
+      <c r="J16" s="73" t="s">
+        <v>82</v>
       </c>
       <c r="K16" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="L16" s="15" t="s">
-        <v>83</v>
+        <v>99</v>
+      </c>
+      <c r="L16" s="73" t="s">
+        <v>82</v>
       </c>
       <c r="M16" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>83</v>
+        <v>99</v>
+      </c>
+      <c r="N16" s="73" t="s">
+        <v>82</v>
       </c>
       <c r="O16" s="42" t="s">
         <v>64</v>
@@ -3704,6 +3761,65 @@
         <v>104</v>
       </c>
       <c r="S16" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="42">
+        <v>30</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="2">
+        <v>100</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="M17" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="O17" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="P17" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q17" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="R17" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S17" s="42" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Respiration rate only goes to zero with a sedative for "over sedation' or when sedation = 1.0 and stays there. The CO2 setpoints that trigger respiration changes are modified by sedation level now. Need to update drug methodology still.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngineStable\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C569540-7DCA-4F52-88EA-07A31D239136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09F0557-AEEC-48C8-8B47-2BDF9CF8705D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="184">
   <si>
     <t>Event</t>
   </si>
@@ -289,9 +289,6 @@
     <t xml:space="preserve">NC or Increase @cite Morgan2006Clinical p192-7, @cite PaulGBarash2009 p285; 5-10% Increase @cite dukeSME   </t>
   </si>
   <si>
-    <t xml:space="preserve">NC @cite Morgan2006Clinical p200; NC @cite dukeSME     </t>
-  </si>
-  <si>
     <t xml:space="preserve">NC @cite PaulGBarash2009 p299; NC @cite dukeSME     </t>
   </si>
   <si>
@@ -301,9 +298,6 @@
     <t xml:space="preserve">Moderate Decrease @cite Morgan2006Clinical p200; 15-25% Decrease @cite dukeSME    </t>
   </si>
   <si>
-    <t xml:space="preserve">Marked Decrease @cite Morgan2006Clinical p200; 25-40% Decrease @cite dukeSME    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Stable @cite Morgan2006Clinical p192-7, @cite PaulGBarash2009 p277;  5-10% Decrease @cite dukeSME  </t>
   </si>
   <si>
@@ -313,18 +307,12 @@
     <t xml:space="preserve">Mild Decrease @cite Morgan2006Clinical p200; 25-50% Decrease @cite dukeSME     </t>
   </si>
   <si>
-    <t xml:space="preserve">Moderate Decrease @cite Morgan2006Clinical p200; Marked Decrease To 0 @cite dukeSME    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Marked Decrease @cite Morgan2006Clinical p200; 15-25% Decrease @cite dukeSME   </t>
   </si>
   <si>
     <t xml:space="preserve">Decrease @cite Morgan2006Clinical p192-7, @cite PaulGBarash2009 p285; Return to resting physiology @cite dukeSME   </t>
   </si>
   <si>
-    <t xml:space="preserve">Marked Decrease @cite Morgan2006Clinical p200; 100% Decrease @cite dukeSME    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Goes to Zero @cite Morgan2006Clinical p224; Goes to Zero @cite dukeSME     </t>
   </si>
   <si>
@@ -593,6 +581,21 @@
   </si>
   <si>
     <t>Mild Decrease @cite Ghiasi2021lorazepam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderate Decrease @cite Morgan2006Clinical p200; Slight decrease @cite Tulen1991dose    </t>
+  </si>
+  <si>
+    <t>Slight Increase, Decrease in Tidal Volume @cite Lee2011effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Significant Decrease @cite Kanaya2003differential </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marked Decrease @cite Morgan2006Clinical p200; 25-40% Significant Decrease @cite Kanaya2003differential  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marked Decrease @cite Morgan2006Clinical p200; 25-40% Significant Decrease @cite Kanaya2003differential </t>
   </si>
 </sst>
 </file>
@@ -1780,7 +1783,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,19 +1819,19 @@
         <v>52</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G1" s="50" t="s">
         <v>52</v>
       </c>
       <c r="H1" s="44" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I1" s="50" t="s">
         <v>52</v>
       </c>
       <c r="J1" s="43" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K1" s="52" t="s">
         <v>52</v>
@@ -1889,13 +1892,13 @@
         <v>5</v>
       </c>
       <c r="G3" s="67" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H3" s="8">
         <v>0</v>
       </c>
       <c r="I3" s="70" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J3" s="9">
         <v>0</v>
@@ -1913,13 +1916,13 @@
         <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C4" s="66" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E4" s="65" t="s">
         <v>54</v>
@@ -1928,13 +1931,13 @@
         <v>5</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H4" s="8">
         <v>0</v>
       </c>
       <c r="I4" s="72" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J4" s="9">
         <v>0</v>
@@ -1958,7 +1961,7 @@
         <v>52</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E5" s="65" t="s">
         <v>54</v>
@@ -1967,13 +1970,13 @@
         <v>4</v>
       </c>
       <c r="G5" s="67" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
       </c>
       <c r="I5" s="70" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J5" s="9">
         <v>0</v>
@@ -2006,13 +2009,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="67" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
       </c>
       <c r="I6" s="70" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J6" s="9">
         <v>0</v>
@@ -2045,13 +2048,13 @@
         <v>4</v>
       </c>
       <c r="G7" s="67" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H7" s="8">
         <v>1</v>
       </c>
       <c r="I7" s="70" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J7" s="9">
         <v>0</v>
@@ -2069,13 +2072,13 @@
         <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C8" s="66" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E8" s="65" t="s">
         <v>54</v>
@@ -2084,13 +2087,13 @@
         <v>5</v>
       </c>
       <c r="G8" s="72" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H8" s="8">
         <v>0</v>
       </c>
       <c r="I8" s="72" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J8" s="9">
         <v>0</v>
@@ -2123,13 +2126,13 @@
         <v>5</v>
       </c>
       <c r="G9" s="68" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H9" s="8">
         <v>0</v>
       </c>
       <c r="I9" s="71" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J9" s="9">
         <v>0</v>
@@ -2162,13 +2165,13 @@
         <v>5</v>
       </c>
       <c r="G10" s="68" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H10" s="8">
         <v>0</v>
       </c>
       <c r="I10" s="71" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J10" s="9">
         <v>0</v>
@@ -2192,7 +2195,7 @@
         <v>52</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E11" s="65" t="s">
         <v>54</v>
@@ -2201,13 +2204,13 @@
         <v>5</v>
       </c>
       <c r="G11" s="68" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H11" s="8">
         <v>0</v>
       </c>
       <c r="I11" s="71" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J11" s="9">
         <v>0</v>
@@ -2227,7 +2230,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E12" s="65" t="s">
         <v>54</v>
@@ -2236,13 +2239,13 @@
         <v>5</v>
       </c>
       <c r="G12" s="68" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H12" s="8">
         <v>0</v>
       </c>
       <c r="I12" s="71" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J12" s="9">
         <v>0</v>
@@ -2271,13 +2274,13 @@
         <v>5</v>
       </c>
       <c r="G13" s="69" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H13" s="8">
         <v>0</v>
       </c>
       <c r="I13" s="72" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J13" s="9">
         <v>0</v>
@@ -2303,19 +2306,19 @@
         <v>54</v>
       </c>
       <c r="F14" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14" s="69" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H14" s="16">
         <v>0</v>
       </c>
       <c r="I14" s="72" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J14" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="51" t="s">
         <v>56</v>
@@ -2341,13 +2344,13 @@
         <v>2</v>
       </c>
       <c r="G15" s="69" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H15" s="8">
         <v>0</v>
       </c>
       <c r="I15" s="72" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J15" s="9">
         <v>3</v>
@@ -2376,13 +2379,13 @@
         <v>5</v>
       </c>
       <c r="G16" s="69" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H16" s="8">
         <v>0</v>
       </c>
       <c r="I16" s="72" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J16" s="9">
         <v>0</v>
@@ -2400,28 +2403,28 @@
         <v>52</v>
       </c>
       <c r="D17" s="59" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E17" s="57" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="60">
         <f>SUM(F3:F16)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G17" s="61" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H17" s="62">
         <f>SUM(H3:H16)</f>
         <v>2</v>
       </c>
       <c r="I17" s="61" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J17" s="63">
         <f>SUM(J3:J16)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K17" s="64" t="s">
         <v>56</v>
@@ -2569,7 +2572,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>52</v>
@@ -2617,7 +2620,7 @@
         <v>52</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="W2" s="21" t="s">
         <v>52</v>
@@ -2726,7 +2729,7 @@
         <v>61</v>
       </c>
       <c r="K4" s="40" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L4" s="73" t="s">
         <v>62</v>
@@ -2753,13 +2756,13 @@
         <v>64</v>
       </c>
       <c r="T4" s="26" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="U4" s="40" t="s">
         <v>64</v>
       </c>
       <c r="V4" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="W4" s="40" t="s">
         <v>56</v>
@@ -2850,7 +2853,7 @@
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection activeCell="F4" sqref="F4"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:S17"/>
+      <selection pane="topRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,7 +2899,7 @@
         <v>52</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G2" s="42" t="s">
         <v>52</v>
@@ -3050,7 +3053,7 @@
         <v>64</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S4" s="42" t="s">
         <v>56</v>
@@ -3061,7 +3064,7 @@
         <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>52</v>
@@ -3085,31 +3088,31 @@
         <v>54</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K5" s="42" t="s">
         <v>64</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="M5" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O5" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Q5" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R5" s="14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="S5" s="42" t="s">
         <v>56</v>
@@ -3162,13 +3165,13 @@
         <v>64</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q6" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R6" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S6" s="42" t="s">
         <v>56</v>
@@ -3212,7 +3215,7 @@
         <v>77</v>
       </c>
       <c r="M7" s="42" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>77</v>
@@ -3221,13 +3224,13 @@
         <v>64</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q7" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S7" s="42" t="s">
         <v>56</v>
@@ -3238,13 +3241,13 @@
         <v>52</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E8" s="42" t="s">
         <v>52</v>
@@ -3262,31 +3265,31 @@
         <v>54</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="K8" s="42" t="s">
         <v>64</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="M8" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="O8" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="Q8" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="S8" s="42" t="s">
         <v>56</v>
@@ -3327,25 +3330,25 @@
         <v>64</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M9" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O9" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>89</v>
+        <v>179</v>
       </c>
       <c r="Q9" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="S9" s="42" t="s">
         <v>56</v>
@@ -3386,25 +3389,25 @@
         <v>64</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M10" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O10" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Q10" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R10" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="S10" s="42" t="s">
         <v>56</v>
@@ -3451,19 +3454,19 @@
         <v>64</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O11" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P11" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q11" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S11" s="42" t="s">
         <v>56</v>
@@ -3516,13 +3519,13 @@
         <v>64</v>
       </c>
       <c r="P12" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q12" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R12" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="S12" s="42" t="s">
         <v>56</v>
@@ -3646,7 +3649,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>52</v>
       </c>
@@ -3672,34 +3675,34 @@
         <v>100</v>
       </c>
       <c r="I15" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="J15" s="73" t="s">
-        <v>81</v>
+        <v>54</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="K15" s="42" t="s">
         <v>64</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="M15" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
       <c r="O15" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P15" s="15" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="Q15" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R15" s="13" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="S15" s="42" t="s">
         <v>56</v>
@@ -3734,31 +3737,31 @@
         <v>59</v>
       </c>
       <c r="J16" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K16" s="42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L16" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M16" s="42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N16" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O16" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P16" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="Q16" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R16" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="S16" s="42" t="s">
         <v>56</v>
@@ -3769,7 +3772,7 @@
         <v>52</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>52</v>
@@ -3793,31 +3796,31 @@
         <v>54</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" s="42" t="s">
         <v>64</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M17" s="42" t="s">
         <v>64</v>
       </c>
       <c r="N17" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O17" s="42" t="s">
         <v>64</v>
       </c>
       <c r="P17" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="Q17" s="42" t="s">
         <v>64</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="S17" s="42" t="s">
         <v>56</v>
@@ -3880,61 +3883,61 @@
         <v>52</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="O2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="I2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="Q2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="K2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="S2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="M2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="O2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="S2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="U2" s="21" t="s">
         <v>52</v>
@@ -4010,7 +4013,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>52</v>
@@ -4022,10 +4025,10 @@
         <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H4" s="12">
         <v>0.76100000000000001</v>
@@ -4034,7 +4037,7 @@
         <v>56</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K4" s="42" t="s">
         <v>54</v>
@@ -4046,10 +4049,10 @@
         <v>56</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O4" s="42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P4" s="12">
         <v>118</v>
@@ -4058,10 +4061,10 @@
         <v>56</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="T4" s="12">
         <v>72</v>
@@ -4075,7 +4078,7 @@
         <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>52</v>
@@ -4087,7 +4090,7 @@
         <v>52</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G5" s="42" t="s">
         <v>54</v>
@@ -4099,7 +4102,7 @@
         <v>56</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="K5" s="42" t="s">
         <v>54</v>
@@ -4111,7 +4114,7 @@
         <v>56</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="O5" s="42" t="s">
         <v>54</v>
@@ -4123,7 +4126,7 @@
         <v>56</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="S5" s="42" t="s">
         <v>54</v>
@@ -4140,7 +4143,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>52</v>
@@ -4152,7 +4155,7 @@
         <v>52</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G6" s="42" t="s">
         <v>54</v>
@@ -4164,7 +4167,7 @@
         <v>56</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K6" s="42" t="s">
         <v>54</v>
@@ -4176,7 +4179,7 @@
         <v>56</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="O6" s="42" t="s">
         <v>54</v>
@@ -4188,7 +4191,7 @@
         <v>56</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="S6" s="42" t="s">
         <v>54</v>
@@ -4205,7 +4208,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>52</v>
@@ -4217,7 +4220,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G7" s="42" t="s">
         <v>54</v>
@@ -4229,7 +4232,7 @@
         <v>56</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K7" s="42" t="s">
         <v>54</v>
@@ -4241,7 +4244,7 @@
         <v>56</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O7" s="42" t="s">
         <v>54</v>
@@ -4253,7 +4256,7 @@
         <v>56</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="S7" s="42" t="s">
         <v>54</v>
@@ -4270,7 +4273,7 @@
         <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>52</v>
@@ -4282,7 +4285,7 @@
         <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G8" s="42" t="s">
         <v>54</v>
@@ -4294,7 +4297,7 @@
         <v>56</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K8" s="42" t="s">
         <v>54</v>
@@ -4306,7 +4309,7 @@
         <v>56</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="O8" s="42" t="s">
         <v>54</v>
@@ -4318,7 +4321,7 @@
         <v>56</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="S8" s="42" t="s">
         <v>54</v>
@@ -4377,61 +4380,61 @@
         <v>52</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="O2" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="I2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="M2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="O2" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="Q2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="S2" s="42" t="s">
         <v>52</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="U2" s="21" t="s">
         <v>52</v>
@@ -4507,7 +4510,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>52</v>
@@ -4519,10 +4522,10 @@
         <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H4" s="12">
         <v>6</v>
@@ -4531,7 +4534,7 @@
         <v>56</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K4" s="42" t="s">
         <v>54</v>
@@ -4543,7 +4546,7 @@
         <v>56</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="O4" s="42" t="s">
         <v>54</v>
@@ -4555,7 +4558,7 @@
         <v>56</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="S4" s="42" t="s">
         <v>54</v>
@@ -4572,7 +4575,7 @@
         <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>52</v>
@@ -4584,7 +4587,7 @@
         <v>52</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G5" s="42" t="s">
         <v>54</v>
@@ -4596,10 +4599,10 @@
         <v>56</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="K5" s="42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="L5" s="12">
         <v>-2</v>
@@ -4608,7 +4611,7 @@
         <v>56</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="O5" s="42" t="s">
         <v>54</v>
@@ -4620,7 +4623,7 @@
         <v>56</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="S5" s="42" t="s">
         <v>54</v>
@@ -4637,7 +4640,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>52</v>
@@ -4649,7 +4652,7 @@
         <v>52</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G6" s="42" t="s">
         <v>54</v>
@@ -4661,7 +4664,7 @@
         <v>56</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K6" s="42" t="s">
         <v>59</v>
@@ -4673,10 +4676,10 @@
         <v>56</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O6" s="42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P6" s="12">
         <v>13</v>
@@ -4685,7 +4688,7 @@
         <v>56</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="S6" s="42" t="s">
         <v>54</v>
@@ -4702,7 +4705,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>52</v>
@@ -4714,7 +4717,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G7" s="42" t="s">
         <v>54</v>
@@ -4726,7 +4729,7 @@
         <v>56</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="K7" s="42" t="s">
         <v>59</v>
@@ -4738,10 +4741,10 @@
         <v>56</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P7" s="12">
         <v>17</v>
@@ -4750,7 +4753,7 @@
         <v>56</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="S7" s="42" t="s">
         <v>54</v>
@@ -4833,37 +4836,37 @@
         <v>52</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>52</v>
       </c>
       <c r="H2" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="Q2" s="21" t="s">
         <v>52</v>
@@ -4927,7 +4930,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>52</v>
@@ -4951,25 +4954,25 @@
         <v>54</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K4" s="40" t="s">
         <v>64</v>
       </c>
       <c r="L4" s="75" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="M4" s="40" t="s">
         <v>64</v>
       </c>
       <c r="N4" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="O4" s="40" t="s">
         <v>64</v>
       </c>
       <c r="P4" s="25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Q4" s="40" t="s">
         <v>56</v>

</xml_diff>